<commit_message>
Limit QC to current MSL; implement type species fixes for 3 genera.
</commit_message>
<xml_diff>
--- a/7e.REPORT.QC_check_for_genera_with_type_species_issues.sql.xlsx
+++ b/7e.REPORT.QC_check_for_genera_with_type_species_issues.sql.xlsx
@@ -24,56 +24,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="45">
   <si>
     <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Demerecviridae;Novosibvirus</t>
   </si>
   <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Autographiviridae;Limelightvirus</t>
-  </si>
-  <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Autographiviridae;Waewaevirus</t>
-  </si>
-  <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Drexlerviridae;Gyeonggidovirus</t>
-  </si>
-  <si>
     <t>Riboviria;Orthornavirae;Pisuviricota;Pisoniviricetes;Nidovirales;Tornidovirineae;Tobaniviridae;Serpentovirinae;Pregotovirus</t>
   </si>
   <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Autographiviridae;Unyawo</t>
-  </si>
-  <si>
-    <t>Riboviria;Orthornavirae;Negarnaviricota;Polyploviricotina;Ellioviricetes;Bunyavirales;Phenuiviridae;Laulavirus</t>
-  </si>
-  <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Myoviridae;Thornevirus</t>
-  </si>
-  <si>
     <t>Riboviria;Orthornavirae;Pisuviricota;Pisoniviricetes;Picornavirales;Secoviridae;Sadwavirus</t>
   </si>
   <si>
-    <t>Duplodnaviria;Heunggongvirae;Uroviricota;Caudoviricetes;Caudovirales;Autographiviridae;Tiilvirus</t>
-  </si>
-  <si>
-    <t>Caudovirales;Myoviridae;Thornevirus</t>
-  </si>
-  <si>
-    <t>Riboviria;Negarnaviricota;Polyploviricotina;Ellioviricetes;Bunyavirales;Phenuiviridae;Laulavirus</t>
-  </si>
-  <si>
     <t>Caudovirales;Siphoviridae;T5likevirus</t>
   </si>
   <si>
     <t>Rudiviridae;Rudivirus</t>
   </si>
   <si>
-    <t>Caudovirales;Myoviridae;T4-like phages</t>
-  </si>
-  <si>
-    <t>Polydnaviridae;Brachovirus</t>
-  </si>
-  <si>
     <t>Picornaviridae;Unnamed genus</t>
   </si>
   <si>
@@ -86,9 +53,6 @@
     <t>Retroviridae;Spumavirus</t>
   </si>
   <si>
-    <t>Orthomyxoviridae;Influenza type C viruses</t>
-  </si>
-  <si>
     <t>Retroviridae;HTL-BLV group</t>
   </si>
   <si>
@@ -143,9 +107,6 @@
     <t>ERROR: too MANY type species: each genus should have EXACTLY 1 type species</t>
   </si>
   <si>
-    <t>ERROR: genus has only 1 species, but it is NOT a type species. A genus must have have EXACTLY 1 species</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -158,27 +119,6 @@
     <t>Novosibvirus</t>
   </si>
   <si>
-    <t>Limelightvirus</t>
-  </si>
-  <si>
-    <t>Tiilvirus</t>
-  </si>
-  <si>
-    <t>Unyawo</t>
-  </si>
-  <si>
-    <t>Waewaevirus</t>
-  </si>
-  <si>
-    <t>Gyeonggidovirus</t>
-  </si>
-  <si>
-    <t>Thornevirus</t>
-  </si>
-  <si>
-    <t>Laulavirus</t>
-  </si>
-  <si>
     <t>T5likevirus</t>
   </si>
   <si>
@@ -188,12 +128,6 @@
     <t>ERROR: genera should have EXACTLY 1 species</t>
   </si>
   <si>
-    <t>T4-like phages</t>
-  </si>
-  <si>
-    <t>Brachovirus</t>
-  </si>
-  <si>
     <t>Unnamed genus</t>
   </si>
   <si>
@@ -210,9 +144,6 @@
   </si>
   <si>
     <t>Mammalian type C retrovirus group</t>
-  </si>
-  <si>
-    <t>Influenza type C viruses</t>
   </si>
   <si>
     <t>Lentivirus</t>
@@ -612,11 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,43 +564,43 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -678,21 +609,21 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>4</v>
@@ -701,12 +632,12 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>35</v>
@@ -715,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -724,689 +655,689 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C6">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="C11">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
       <c r="F11">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C16">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="C18">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
       <c r="F18">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="C21">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
       <c r="F21">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="C24">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
       <c r="F24">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25">
         <v>13</v>
       </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25">
-        <v>7</v>
-      </c>
       <c r="G25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F26">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
         <v>36</v>
       </c>
-      <c r="C27">
-        <v>11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
-      </c>
       <c r="F27">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
         <v>36</v>
       </c>
-      <c r="C29">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" t="s">
-        <v>61</v>
-      </c>
       <c r="F29">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F31">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
         <v>36</v>
       </c>
-      <c r="C32">
-        <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" t="s">
-        <v>64</v>
-      </c>
       <c r="F32">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="F33">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
         <v>36</v>
       </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" t="s">
-        <v>58</v>
-      </c>
       <c r="F34">
         <v>24</v>
       </c>
@@ -1414,21 +1345,21 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="F35">
         <v>13</v>
@@ -1437,444 +1368,53 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="F37">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" t="s">
-        <v>65</v>
-      </c>
-      <c r="F38">
-        <v>7</v>
-      </c>
-      <c r="G38">
-        <v>3</v>
-      </c>
-      <c r="H38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39">
-        <v>13</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40">
-        <v>7</v>
-      </c>
-      <c r="G40">
-        <v>3</v>
-      </c>
-      <c r="H40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41">
-        <v>24</v>
-      </c>
-      <c r="G41">
-        <v>3</v>
-      </c>
-      <c r="H41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42">
-        <v>8</v>
-      </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42">
-        <v>13</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43">
-        <v>3</v>
-      </c>
-      <c r="H43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44">
-        <v>24</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="H44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" t="s">
-        <v>66</v>
-      </c>
-      <c r="F45">
-        <v>13</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" t="s">
-        <v>58</v>
-      </c>
-      <c r="F46">
-        <v>24</v>
-      </c>
-      <c r="G46">
-        <v>3</v>
-      </c>
-      <c r="H46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>25</v>
-      </c>
-      <c r="E47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47">
-        <v>5</v>
-      </c>
-      <c r="G47">
-        <v>3</v>
-      </c>
-      <c r="H47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48">
-        <v>13</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F49">
-        <v>24</v>
-      </c>
-      <c r="G49">
-        <v>3</v>
-      </c>
-      <c r="H49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" t="s">
-        <v>66</v>
-      </c>
-      <c r="F50">
-        <v>13</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" t="s">
-        <v>58</v>
-      </c>
-      <c r="F51">
-        <v>24</v>
-      </c>
-      <c r="G51">
-        <v>3</v>
-      </c>
-      <c r="H51" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
-        <v>26</v>
-      </c>
-      <c r="E52" t="s">
-        <v>66</v>
-      </c>
-      <c r="F52">
-        <v>13</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>28</v>
-      </c>
-      <c r="E53" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53">
-        <v>5</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>29</v>
-      </c>
-      <c r="E54" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54">
-        <v>3</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>